<commit_message>
Aggiunta messaggi mancanti e corretti errori grammaticali
</commit_message>
<xml_diff>
--- a/Secondo use case.xlsx
+++ b/Secondo use case.xlsx
@@ -39,18 +39,9 @@
     <t>Entry conditions</t>
   </si>
   <si>
-    <t>the system register the request and 10 minutes before the scheduled deparures send the request's and the user's basic information to the first taxi driver in the zone</t>
-  </si>
-  <si>
-    <t>the taxi driver accepts the request</t>
-  </si>
-  <si>
     <t xml:space="preserve">The user requests the taxi specifying the time and the position </t>
   </si>
   <si>
-    <t>the system removes the taxi driver from the queue and send to the user the reminder of the incoming taxi and the expected waiting time</t>
-  </si>
-  <si>
     <t>The taxi driver goes to pic up the user and brings him/her to the destination.</t>
   </si>
   <si>
@@ -70,6 +61,15 @@
   </si>
   <si>
     <t xml:space="preserve">The System put the taxi driver in the last position of his/her actual zone's queue  </t>
+  </si>
+  <si>
+    <t>The taxi driver accepts the request</t>
+  </si>
+  <si>
+    <t>The system register the request and 10 minutes before the scheduled deparure send the request's and the user's basic information to the first taxi driver in the zone</t>
+  </si>
+  <si>
+    <t>The system removes the taxi driver from the queue and send to the user the reminder of the incoming taxi and the expected waiting time</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -442,53 +442,53 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>